<commit_message>
made setup and teardown functions for CsvReaderTests creating/destroying fake datasets
</commit_message>
<xml_diff>
--- a/picturae_import/picturae_csv/2023-6-28/picturae_folder(6_24_2023).xlsx
+++ b/picturae_import/picturae_csv/2023-6-28/picturae_folder(6_24_2023).xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdelaroca/Documents/sandbox_db/specify-sandbox/web-asset-server/image_client/picturae_import/picturae_csv/6_24_2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdelaroca/Documents/sandbox_db/specify-sandbox/web-asset-server/image_client/picturae_import/picturae_csv/2023-6-28/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B2ED0D38-951E-BB4C-A032-06DF43D63E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8657A8D-6F2D-0740-8D5E-78B5BEF30498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="1880" windowWidth="27240" windowHeight="16440"/>
+    <workbookView xWindow="11040" yWindow="3460" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="picturae_folder(6_24_2023)" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -34,9 +34,6 @@
     <t>folder_barcode</t>
   </si>
   <si>
-    <t>speciemen barcode</t>
-  </si>
-  <si>
     <t>filed_as_family</t>
   </si>
   <si>
@@ -287,12 +284,15 @@
   </si>
   <si>
     <t>Cover 123480_1.jpg</t>
+  </si>
+  <si>
+    <t>speciemen_barcode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1126,11 +1126,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D50"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1149,76 +1149,76 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
@@ -1226,16 +1226,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -1248,25 +1248,25 @@
         <v>54192</v>
       </c>
       <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
         <v>28</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>29</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>30</v>
       </c>
-      <c r="N2" t="s">
-        <v>31</v>
-      </c>
       <c r="U2" t="b">
         <v>0</v>
       </c>
       <c r="AA2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
@@ -1274,16 +1274,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -1296,25 +1296,25 @@
         <v>54192</v>
       </c>
       <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
         <v>28</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>29</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>30</v>
       </c>
-      <c r="N3" t="s">
-        <v>31</v>
-      </c>
       <c r="U3" t="b">
         <v>0</v>
       </c>
       <c r="AA3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
@@ -1322,16 +1322,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -1344,25 +1344,25 @@
         <v>54192</v>
       </c>
       <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" t="s">
         <v>28</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>29</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>30</v>
       </c>
-      <c r="N4" t="s">
-        <v>31</v>
-      </c>
       <c r="U4" t="b">
         <v>0</v>
       </c>
       <c r="AA4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
@@ -1370,16 +1370,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -1392,25 +1392,25 @@
         <v>54192</v>
       </c>
       <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
         <v>28</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>29</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>30</v>
       </c>
-      <c r="N5" t="s">
-        <v>31</v>
-      </c>
       <c r="U5" t="b">
         <v>0</v>
       </c>
       <c r="AA5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
@@ -1418,16 +1418,16 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
@@ -1440,25 +1440,25 @@
         <v>54192</v>
       </c>
       <c r="J6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" t="s">
         <v>28</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>29</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>30</v>
       </c>
-      <c r="N6" t="s">
-        <v>31</v>
-      </c>
       <c r="U6" t="b">
         <v>0</v>
       </c>
       <c r="AA6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
@@ -1466,16 +1466,16 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
@@ -1488,25 +1488,25 @@
         <v>54192</v>
       </c>
       <c r="J7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" t="s">
         <v>28</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>29</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>30</v>
       </c>
-      <c r="N7" t="s">
-        <v>31</v>
-      </c>
       <c r="U7" t="b">
         <v>0</v>
       </c>
       <c r="AA7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
@@ -1514,16 +1514,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
@@ -1536,25 +1536,25 @@
         <v>54192</v>
       </c>
       <c r="J8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" t="s">
         <v>28</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>29</v>
       </c>
-      <c r="L8" t="s">
+      <c r="N8" t="s">
         <v>30</v>
       </c>
-      <c r="N8" t="s">
-        <v>31</v>
-      </c>
       <c r="U8" t="b">
         <v>0</v>
       </c>
       <c r="AA8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
@@ -1562,16 +1562,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
@@ -1584,25 +1584,25 @@
         <v>54192</v>
       </c>
       <c r="J9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" t="s">
         <v>28</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>29</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N9" t="s">
         <v>30</v>
       </c>
-      <c r="N9" t="s">
-        <v>31</v>
-      </c>
       <c r="U9" t="b">
         <v>0</v>
       </c>
       <c r="AA9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
@@ -1610,16 +1610,16 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
@@ -1632,25 +1632,25 @@
         <v>54192</v>
       </c>
       <c r="J10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" t="s">
         <v>28</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>29</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>30</v>
       </c>
-      <c r="N10" t="s">
-        <v>31</v>
-      </c>
       <c r="U10" t="b">
         <v>0</v>
       </c>
       <c r="AA10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
@@ -1658,16 +1658,16 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
@@ -1680,25 +1680,25 @@
         <v>54192</v>
       </c>
       <c r="J11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" t="s">
         <v>28</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>29</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
         <v>30</v>
       </c>
-      <c r="N11" t="s">
-        <v>31</v>
-      </c>
       <c r="U11" t="b">
         <v>0</v>
       </c>
       <c r="AA11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
@@ -1706,16 +1706,16 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
@@ -1728,25 +1728,25 @@
         <v>54192</v>
       </c>
       <c r="J12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" t="s">
         <v>28</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>29</v>
       </c>
-      <c r="L12" t="s">
+      <c r="N12" t="s">
         <v>30</v>
       </c>
-      <c r="N12" t="s">
-        <v>31</v>
-      </c>
       <c r="U12" t="b">
         <v>0</v>
       </c>
       <c r="AA12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
@@ -1754,16 +1754,16 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
@@ -1776,25 +1776,25 @@
         <v>54192</v>
       </c>
       <c r="J13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" t="s">
         <v>28</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>29</v>
       </c>
-      <c r="L13" t="s">
+      <c r="N13" t="s">
         <v>30</v>
       </c>
-      <c r="N13" t="s">
-        <v>31</v>
-      </c>
       <c r="U13" t="b">
         <v>0</v>
       </c>
       <c r="AA13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
@@ -1802,16 +1802,16 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
@@ -1824,25 +1824,25 @@
         <v>54192</v>
       </c>
       <c r="J14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" t="s">
         <v>28</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>29</v>
       </c>
-      <c r="L14" t="s">
+      <c r="N14" t="s">
         <v>30</v>
       </c>
-      <c r="N14" t="s">
-        <v>31</v>
-      </c>
       <c r="U14" t="b">
         <v>0</v>
       </c>
       <c r="AA14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
@@ -1850,16 +1850,16 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
@@ -1872,25 +1872,25 @@
         <v>54192</v>
       </c>
       <c r="J15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" t="s">
         <v>28</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>29</v>
       </c>
-      <c r="L15" t="s">
+      <c r="N15" t="s">
         <v>30</v>
       </c>
-      <c r="N15" t="s">
-        <v>31</v>
-      </c>
       <c r="U15" t="b">
         <v>0</v>
       </c>
       <c r="AA15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
@@ -1898,16 +1898,16 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
@@ -1920,25 +1920,25 @@
         <v>54192</v>
       </c>
       <c r="J16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" t="s">
         <v>28</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>29</v>
       </c>
-      <c r="L16" t="s">
+      <c r="N16" t="s">
         <v>30</v>
       </c>
-      <c r="N16" t="s">
-        <v>31</v>
-      </c>
       <c r="U16" t="b">
         <v>0</v>
       </c>
       <c r="AA16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.2">
@@ -1946,16 +1946,16 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
@@ -1968,25 +1968,25 @@
         <v>54192</v>
       </c>
       <c r="J17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" t="s">
         <v>28</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>29</v>
       </c>
-      <c r="L17" t="s">
+      <c r="N17" t="s">
         <v>30</v>
       </c>
-      <c r="N17" t="s">
-        <v>31</v>
-      </c>
       <c r="U17" t="b">
         <v>0</v>
       </c>
       <c r="AA17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.2">
@@ -1994,16 +1994,16 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
@@ -2016,25 +2016,25 @@
         <v>54192</v>
       </c>
       <c r="J18" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" t="s">
         <v>28</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>29</v>
       </c>
-      <c r="L18" t="s">
+      <c r="N18" t="s">
         <v>30</v>
       </c>
-      <c r="N18" t="s">
-        <v>31</v>
-      </c>
       <c r="U18" t="b">
         <v>0</v>
       </c>
       <c r="AA18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.2">
@@ -2042,16 +2042,16 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
@@ -2064,25 +2064,25 @@
         <v>54192</v>
       </c>
       <c r="J19" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" t="s">
         <v>28</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>29</v>
       </c>
-      <c r="L19" t="s">
+      <c r="N19" t="s">
         <v>30</v>
       </c>
-      <c r="N19" t="s">
-        <v>31</v>
-      </c>
       <c r="U19" t="b">
         <v>0</v>
       </c>
       <c r="AA19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.2">
@@ -2090,16 +2090,16 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F20" t="b">
         <v>1</v>
@@ -2112,25 +2112,25 @@
         <v>54192</v>
       </c>
       <c r="J20" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" t="s">
         <v>28</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>29</v>
       </c>
-      <c r="L20" t="s">
+      <c r="N20" t="s">
         <v>30</v>
       </c>
-      <c r="N20" t="s">
-        <v>31</v>
-      </c>
       <c r="U20" t="b">
         <v>0</v>
       </c>
       <c r="AA20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.2">
@@ -2138,16 +2138,16 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21" t="b">
         <v>1</v>
@@ -2160,25 +2160,25 @@
         <v>54192</v>
       </c>
       <c r="J21" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" t="s">
         <v>28</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>29</v>
       </c>
-      <c r="L21" t="s">
+      <c r="N21" t="s">
         <v>30</v>
       </c>
-      <c r="N21" t="s">
-        <v>31</v>
-      </c>
       <c r="U21" t="b">
         <v>0</v>
       </c>
       <c r="AA21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
@@ -2186,16 +2186,16 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F22" t="b">
         <v>1</v>
@@ -2208,25 +2208,25 @@
         <v>54192</v>
       </c>
       <c r="J22" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" t="s">
         <v>28</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>29</v>
       </c>
-      <c r="L22" t="s">
+      <c r="N22" t="s">
         <v>30</v>
       </c>
-      <c r="N22" t="s">
-        <v>31</v>
-      </c>
       <c r="U22" t="b">
         <v>0</v>
       </c>
       <c r="AA22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
@@ -2234,16 +2234,16 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F23" t="b">
         <v>1</v>
@@ -2256,25 +2256,25 @@
         <v>54192</v>
       </c>
       <c r="J23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" t="s">
         <v>28</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>29</v>
       </c>
-      <c r="L23" t="s">
+      <c r="N23" t="s">
         <v>30</v>
       </c>
-      <c r="N23" t="s">
-        <v>31</v>
-      </c>
       <c r="U23" t="b">
         <v>0</v>
       </c>
       <c r="AA23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
@@ -2282,16 +2282,16 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F24" t="b">
         <v>1</v>
@@ -2304,25 +2304,25 @@
         <v>54192</v>
       </c>
       <c r="J24" t="s">
+        <v>27</v>
+      </c>
+      <c r="K24" t="s">
         <v>28</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>29</v>
       </c>
-      <c r="L24" t="s">
+      <c r="N24" t="s">
         <v>30</v>
       </c>
-      <c r="N24" t="s">
-        <v>31</v>
-      </c>
       <c r="U24" t="b">
         <v>0</v>
       </c>
       <c r="AA24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
@@ -2330,16 +2330,16 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F25" t="b">
         <v>1</v>
@@ -2352,25 +2352,25 @@
         <v>54192</v>
       </c>
       <c r="J25" t="s">
+        <v>27</v>
+      </c>
+      <c r="K25" t="s">
         <v>28</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>29</v>
       </c>
-      <c r="L25" t="s">
+      <c r="N25" t="s">
         <v>30</v>
       </c>
-      <c r="N25" t="s">
-        <v>31</v>
-      </c>
       <c r="U25" t="b">
         <v>0</v>
       </c>
       <c r="AA25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
@@ -2378,16 +2378,16 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F26" t="b">
         <v>1</v>
@@ -2400,25 +2400,25 @@
         <v>54216</v>
       </c>
       <c r="J26" t="s">
+        <v>33</v>
+      </c>
+      <c r="K26" t="s">
         <v>34</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>35</v>
       </c>
-      <c r="L26" t="s">
+      <c r="N26" t="s">
         <v>36</v>
       </c>
-      <c r="N26" t="s">
-        <v>37</v>
-      </c>
       <c r="U26" t="b">
         <v>0</v>
       </c>
       <c r="AA26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
@@ -2426,16 +2426,16 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F27" t="b">
         <v>1</v>
@@ -2448,25 +2448,25 @@
         <v>54216</v>
       </c>
       <c r="J27" t="s">
+        <v>33</v>
+      </c>
+      <c r="K27" t="s">
         <v>34</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>35</v>
       </c>
-      <c r="L27" t="s">
+      <c r="N27" t="s">
         <v>36</v>
       </c>
-      <c r="N27" t="s">
-        <v>37</v>
-      </c>
       <c r="U27" t="b">
         <v>0</v>
       </c>
       <c r="AA27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
@@ -2474,16 +2474,16 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
@@ -2496,25 +2496,25 @@
         <v>54216</v>
       </c>
       <c r="J28" t="s">
+        <v>33</v>
+      </c>
+      <c r="K28" t="s">
         <v>34</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>35</v>
       </c>
-      <c r="L28" t="s">
+      <c r="N28" t="s">
         <v>36</v>
       </c>
-      <c r="N28" t="s">
-        <v>37</v>
-      </c>
       <c r="U28" t="b">
         <v>0</v>
       </c>
       <c r="AA28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
@@ -2522,16 +2522,16 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F29" t="b">
         <v>1</v>
@@ -2544,25 +2544,25 @@
         <v>54216</v>
       </c>
       <c r="J29" t="s">
+        <v>33</v>
+      </c>
+      <c r="K29" t="s">
         <v>34</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>35</v>
       </c>
-      <c r="L29" t="s">
+      <c r="N29" t="s">
         <v>36</v>
       </c>
-      <c r="N29" t="s">
-        <v>37</v>
-      </c>
       <c r="U29" t="b">
         <v>0</v>
       </c>
       <c r="AA29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
@@ -2570,16 +2570,16 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F30" t="b">
         <v>1</v>
@@ -2592,25 +2592,25 @@
         <v>54216</v>
       </c>
       <c r="J30" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" t="s">
         <v>34</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>35</v>
       </c>
-      <c r="L30" t="s">
+      <c r="N30" t="s">
         <v>36</v>
       </c>
-      <c r="N30" t="s">
-        <v>37</v>
-      </c>
       <c r="U30" t="b">
         <v>0</v>
       </c>
       <c r="AA30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
@@ -2618,16 +2618,16 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F31" t="b">
         <v>1</v>
@@ -2640,25 +2640,25 @@
         <v>54216</v>
       </c>
       <c r="J31" t="s">
+        <v>33</v>
+      </c>
+      <c r="K31" t="s">
         <v>34</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>35</v>
       </c>
-      <c r="L31" t="s">
+      <c r="N31" t="s">
         <v>36</v>
       </c>
-      <c r="N31" t="s">
-        <v>37</v>
-      </c>
       <c r="U31" t="b">
         <v>0</v>
       </c>
       <c r="AA31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
@@ -2666,16 +2666,16 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F32" t="b">
         <v>1</v>
@@ -2688,25 +2688,25 @@
         <v>54216</v>
       </c>
       <c r="J32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32" t="s">
         <v>34</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>35</v>
       </c>
-      <c r="L32" t="s">
+      <c r="N32" t="s">
         <v>36</v>
       </c>
-      <c r="N32" t="s">
-        <v>37</v>
-      </c>
       <c r="U32" t="b">
         <v>0</v>
       </c>
       <c r="AA32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.2">
@@ -2714,16 +2714,16 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F33" t="b">
         <v>1</v>
@@ -2736,25 +2736,25 @@
         <v>54216</v>
       </c>
       <c r="J33" t="s">
+        <v>33</v>
+      </c>
+      <c r="K33" t="s">
         <v>34</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>35</v>
       </c>
-      <c r="L33" t="s">
+      <c r="N33" t="s">
         <v>36</v>
       </c>
-      <c r="N33" t="s">
-        <v>37</v>
-      </c>
       <c r="U33" t="b">
         <v>0</v>
       </c>
       <c r="AA33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.2">
@@ -2762,16 +2762,16 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F34" t="b">
         <v>1</v>
@@ -2784,25 +2784,25 @@
         <v>54216</v>
       </c>
       <c r="J34" t="s">
+        <v>33</v>
+      </c>
+      <c r="K34" t="s">
         <v>34</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>35</v>
       </c>
-      <c r="L34" t="s">
+      <c r="N34" t="s">
         <v>36</v>
       </c>
-      <c r="N34" t="s">
-        <v>37</v>
-      </c>
       <c r="U34" t="b">
         <v>0</v>
       </c>
       <c r="AA34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.2">
@@ -2810,16 +2810,16 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F35" t="b">
         <v>1</v>
@@ -2832,25 +2832,25 @@
         <v>54216</v>
       </c>
       <c r="J35" t="s">
+        <v>33</v>
+      </c>
+      <c r="K35" t="s">
         <v>34</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>35</v>
       </c>
-      <c r="L35" t="s">
+      <c r="N35" t="s">
         <v>36</v>
       </c>
-      <c r="N35" t="s">
-        <v>37</v>
-      </c>
       <c r="U35" t="b">
         <v>0</v>
       </c>
       <c r="AA35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.2">
@@ -2858,16 +2858,16 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F36" t="b">
         <v>1</v>
@@ -2880,25 +2880,25 @@
         <v>54216</v>
       </c>
       <c r="J36" t="s">
+        <v>33</v>
+      </c>
+      <c r="K36" t="s">
         <v>34</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>35</v>
       </c>
-      <c r="L36" t="s">
+      <c r="N36" t="s">
         <v>36</v>
       </c>
-      <c r="N36" t="s">
-        <v>37</v>
-      </c>
       <c r="U36" t="b">
         <v>0</v>
       </c>
       <c r="AA36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.2">
@@ -2906,16 +2906,16 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F37" t="b">
         <v>1</v>
@@ -2928,25 +2928,25 @@
         <v>54216</v>
       </c>
       <c r="J37" t="s">
+        <v>33</v>
+      </c>
+      <c r="K37" t="s">
         <v>34</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>35</v>
       </c>
-      <c r="L37" t="s">
+      <c r="N37" t="s">
         <v>36</v>
       </c>
-      <c r="N37" t="s">
-        <v>37</v>
-      </c>
       <c r="U37" t="b">
         <v>0</v>
       </c>
       <c r="AA37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.2">
@@ -2954,16 +2954,16 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F38" t="b">
         <v>1</v>
@@ -2976,25 +2976,25 @@
         <v>54216</v>
       </c>
       <c r="J38" t="s">
+        <v>33</v>
+      </c>
+      <c r="K38" t="s">
         <v>34</v>
       </c>
-      <c r="K38" t="s">
+      <c r="L38" t="s">
         <v>35</v>
       </c>
-      <c r="L38" t="s">
+      <c r="N38" t="s">
         <v>36</v>
       </c>
-      <c r="N38" t="s">
-        <v>37</v>
-      </c>
       <c r="U38" t="b">
         <v>0</v>
       </c>
       <c r="AA38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.2">
@@ -3002,16 +3002,16 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F39" t="b">
         <v>1</v>
@@ -3024,25 +3024,25 @@
         <v>54216</v>
       </c>
       <c r="J39" t="s">
+        <v>33</v>
+      </c>
+      <c r="K39" t="s">
         <v>34</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>35</v>
       </c>
-      <c r="L39" t="s">
+      <c r="N39" t="s">
         <v>36</v>
       </c>
-      <c r="N39" t="s">
-        <v>37</v>
-      </c>
       <c r="U39" t="b">
         <v>0</v>
       </c>
       <c r="AA39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.2">
@@ -3050,16 +3050,16 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F40" t="b">
         <v>1</v>
@@ -3072,25 +3072,25 @@
         <v>54216</v>
       </c>
       <c r="J40" t="s">
+        <v>33</v>
+      </c>
+      <c r="K40" t="s">
         <v>34</v>
       </c>
-      <c r="K40" t="s">
+      <c r="L40" t="s">
         <v>35</v>
       </c>
-      <c r="L40" t="s">
+      <c r="N40" t="s">
         <v>36</v>
       </c>
-      <c r="N40" t="s">
-        <v>37</v>
-      </c>
       <c r="U40" t="b">
         <v>0</v>
       </c>
       <c r="AA40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.2">
@@ -3098,16 +3098,16 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F41" t="b">
         <v>1</v>
@@ -3120,25 +3120,25 @@
         <v>54216</v>
       </c>
       <c r="J41" t="s">
+        <v>33</v>
+      </c>
+      <c r="K41" t="s">
         <v>34</v>
       </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
         <v>35</v>
       </c>
-      <c r="L41" t="s">
+      <c r="N41" t="s">
         <v>36</v>
       </c>
-      <c r="N41" t="s">
-        <v>37</v>
-      </c>
       <c r="U41" t="b">
         <v>0</v>
       </c>
       <c r="AA41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.2">
@@ -3146,16 +3146,16 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F42" t="b">
         <v>1</v>
@@ -3168,25 +3168,25 @@
         <v>54216</v>
       </c>
       <c r="J42" t="s">
+        <v>33</v>
+      </c>
+      <c r="K42" t="s">
         <v>34</v>
       </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
         <v>35</v>
       </c>
-      <c r="L42" t="s">
+      <c r="N42" t="s">
         <v>36</v>
       </c>
-      <c r="N42" t="s">
-        <v>37</v>
-      </c>
       <c r="U42" t="b">
         <v>0</v>
       </c>
       <c r="AA42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.2">
@@ -3194,16 +3194,16 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F43" t="b">
         <v>1</v>
@@ -3216,25 +3216,25 @@
         <v>54216</v>
       </c>
       <c r="J43" t="s">
+        <v>33</v>
+      </c>
+      <c r="K43" t="s">
         <v>34</v>
       </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
         <v>35</v>
       </c>
-      <c r="L43" t="s">
+      <c r="N43" t="s">
         <v>36</v>
       </c>
-      <c r="N43" t="s">
-        <v>37</v>
-      </c>
       <c r="U43" t="b">
         <v>0</v>
       </c>
       <c r="AA43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.2">
@@ -3242,16 +3242,16 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F44" t="b">
         <v>1</v>
@@ -3264,25 +3264,25 @@
         <v>54216</v>
       </c>
       <c r="J44" t="s">
+        <v>33</v>
+      </c>
+      <c r="K44" t="s">
         <v>34</v>
       </c>
-      <c r="K44" t="s">
+      <c r="L44" t="s">
         <v>35</v>
       </c>
-      <c r="L44" t="s">
+      <c r="N44" t="s">
         <v>36</v>
       </c>
-      <c r="N44" t="s">
-        <v>37</v>
-      </c>
       <c r="U44" t="b">
         <v>0</v>
       </c>
       <c r="AA44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.2">
@@ -3290,16 +3290,16 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F45" t="b">
         <v>1</v>
@@ -3312,25 +3312,25 @@
         <v>54216</v>
       </c>
       <c r="J45" t="s">
+        <v>33</v>
+      </c>
+      <c r="K45" t="s">
         <v>34</v>
       </c>
-      <c r="K45" t="s">
+      <c r="L45" t="s">
         <v>35</v>
       </c>
-      <c r="L45" t="s">
+      <c r="N45" t="s">
         <v>36</v>
       </c>
-      <c r="N45" t="s">
-        <v>37</v>
-      </c>
       <c r="U45" t="b">
         <v>0</v>
       </c>
       <c r="AA45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB45" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.2">
@@ -3338,16 +3338,16 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F46" t="b">
         <v>1</v>
@@ -3360,25 +3360,25 @@
         <v>54216</v>
       </c>
       <c r="J46" t="s">
+        <v>33</v>
+      </c>
+      <c r="K46" t="s">
         <v>34</v>
       </c>
-      <c r="K46" t="s">
+      <c r="L46" t="s">
         <v>35</v>
       </c>
-      <c r="L46" t="s">
+      <c r="N46" t="s">
         <v>36</v>
       </c>
-      <c r="N46" t="s">
-        <v>37</v>
-      </c>
       <c r="U46" t="b">
         <v>0</v>
       </c>
       <c r="AA46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.2">
@@ -3386,16 +3386,16 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F47" t="b">
         <v>1</v>
@@ -3408,25 +3408,25 @@
         <v>54216</v>
       </c>
       <c r="J47" t="s">
+        <v>33</v>
+      </c>
+      <c r="K47" t="s">
         <v>34</v>
       </c>
-      <c r="K47" t="s">
+      <c r="L47" t="s">
         <v>35</v>
       </c>
-      <c r="L47" t="s">
+      <c r="N47" t="s">
         <v>36</v>
       </c>
-      <c r="N47" t="s">
-        <v>37</v>
-      </c>
       <c r="U47" t="b">
         <v>0</v>
       </c>
       <c r="AA47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.2">
@@ -3434,16 +3434,16 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F48" t="b">
         <v>1</v>
@@ -3456,25 +3456,25 @@
         <v>54216</v>
       </c>
       <c r="J48" t="s">
+        <v>33</v>
+      </c>
+      <c r="K48" t="s">
         <v>34</v>
       </c>
-      <c r="K48" t="s">
+      <c r="L48" t="s">
         <v>35</v>
       </c>
-      <c r="L48" t="s">
+      <c r="N48" t="s">
         <v>36</v>
       </c>
-      <c r="N48" t="s">
-        <v>37</v>
-      </c>
       <c r="U48" t="b">
         <v>0</v>
       </c>
       <c r="AA48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.2">
@@ -3482,16 +3482,16 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E49" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F49" t="b">
         <v>1</v>
@@ -3504,25 +3504,25 @@
         <v>54216</v>
       </c>
       <c r="J49" t="s">
+        <v>33</v>
+      </c>
+      <c r="K49" t="s">
         <v>34</v>
       </c>
-      <c r="K49" t="s">
+      <c r="L49" t="s">
         <v>35</v>
       </c>
-      <c r="L49" t="s">
+      <c r="N49" t="s">
         <v>36</v>
       </c>
-      <c r="N49" t="s">
-        <v>37</v>
-      </c>
       <c r="U49" t="b">
         <v>0</v>
       </c>
       <c r="AA49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB49" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:28" x14ac:dyDescent="0.2">
@@ -3530,16 +3530,16 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C50" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E50" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F50" t="b">
         <v>1</v>
@@ -3552,25 +3552,25 @@
         <v>54216</v>
       </c>
       <c r="J50" t="s">
+        <v>33</v>
+      </c>
+      <c r="K50" t="s">
         <v>34</v>
       </c>
-      <c r="K50" t="s">
+      <c r="L50" t="s">
         <v>35</v>
       </c>
-      <c r="L50" t="s">
+      <c r="N50" t="s">
         <v>36</v>
       </c>
-      <c r="N50" t="s">
-        <v>37</v>
-      </c>
       <c r="U50" t="b">
         <v>0</v>
       </c>
       <c r="AA50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB50" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added setup function  for colnames tests, wrote skeleton for colname funct, incomplete
</commit_message>
<xml_diff>
--- a/picturae_import/picturae_csv/2023-6-28/picturae_folder(6_24_2023).xlsx
+++ b/picturae_import/picturae_csv/2023-6-28/picturae_folder(6_24_2023).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdelaroca/Documents/sandbox_db/specify-sandbox/web-asset-server/image_client/picturae_import/picturae_csv/2023-6-28/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8657A8D-6F2D-0740-8D5E-78B5BEF30498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF31C6A-E1CE-5D41-9FB8-30F8C9076435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="3460" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="760" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="picturae_folder(6_24_2023)" sheetId="1" r:id="rId1"/>
@@ -286,7 +286,7 @@
     <t>Cover 123480_1.jpg</t>
   </si>
   <si>
-    <t>speciemen_barcode</t>
+    <t>specimen_barcode</t>
   </si>
 </sst>
 </file>
@@ -1129,9 +1129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>